<commit_message>
Remove unnecessary activities and variables
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\Name_Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E30C7FA-6E3B-49FC-9566-EA3A621E261B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -84,24 +84,6 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -118,12 +100,6 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
   </si>
   <si>
     <t>MaxConsecutiveSystemExceptions</t>
@@ -157,9 +133,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -212,10 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -223,7 +196,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -537,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -584,36 +557,18 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
+    <row r="3" spans="1:26" ht="14.4">
+      <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
+    <row r="5" spans="1:26" ht="14.4">
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,7 +1575,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1670,21 +1625,21 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1685,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1696,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1707,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,7 +2737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2800,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Add send mail with results
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\Name_Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E507B7ED-8267-49C0-B9F9-496C160CFBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE935D-DCA5-4C42-8B79-83A5D087B311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="996" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,7 +221,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -538,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -622,14 +621,14 @@
       <c r="A9" t="s">
         <v>43</v>
       </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1630,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>